<commit_message>
pi template logic update
</commit_message>
<xml_diff>
--- a/template/order_pi_template.xlsx
+++ b/template/order_pi_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="27560"/>
+    <workbookView windowWidth="26580" windowHeight="21760"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>NINGBO HARBOR IMPORT &amp; EXPORT CO.,LTD</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">To:   </t>
     </r>
     <r>
@@ -123,6 +129,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>Add:</t>
     </r>
     <r>
@@ -149,6 +161,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
       <t>Tel/Fax:</t>
     </r>
     <r>
@@ -185,13 +203,7 @@
     <t>(FOB Ningbo)</t>
   </si>
   <si>
-    <t>TOTAL:</t>
-  </si>
-  <si>
     <t>TOTAL AMOUNT</t>
-  </si>
-  <si>
-    <t>SAY US DOLLARS THIRTY THOUSAND FOUR HUNDRED AND SEVENTY EIGHT CENTS TEN ONLY.</t>
   </si>
   <si>
     <t>(In Capital Letters)</t>
@@ -330,7 +342,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="_ \¥* #,##0.00_ ;_ \¥* \-#,##0.00_ ;_ \¥* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,13 +452,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -797,7 +802,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -834,65 +839,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -906,6 +852,17 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -926,6 +883,17 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1046,140 +1014,140 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1255,39 +1223,39 @@
     <xf numFmtId="26" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="26" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="26" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="26" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1324,14 +1292,11 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="26" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1393,49 +1358,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>212725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1" descr="logo"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2203450" y="7254875"/>
-          <a:ext cx="2272665" cy="1382395"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1727,10 +1649,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
@@ -1739,7 +1661,7 @@
     <col min="2" max="2" width="34.6057692307692" customWidth="1"/>
     <col min="3" max="3" width="18.6346153846154" customWidth="1"/>
     <col min="4" max="4" width="14.6346153846154" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.3461538461538" customWidth="1"/>
+    <col min="5" max="5" width="25.1634615384615" customWidth="1"/>
     <col min="7" max="7" width="12.7307692307692" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1888,70 +1810,70 @@
       <c r="E15" s="23"/>
       <c r="G15" s="46"/>
     </row>
-    <row r="16" s="1" customFormat="1" ht="15" customHeight="1" spans="1:4">
+    <row r="16" s="1" customFormat="1" ht="15" customHeight="1" spans="1:5">
       <c r="A16" s="25"/>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" s="1" customFormat="1" ht="14" customHeight="1" spans="1:5">
-      <c r="A17" s="27" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="26"/>
+    </row>
+    <row r="17" ht="15" customHeight="1" spans="1:5">
+      <c r="A17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="30"/>
-      <c r="E17" s="48">
-        <f>SUM(E14:E16)</f>
-        <v>0</v>
-      </c>
+      <c r="E17" s="48"/>
     </row>
     <row r="18" ht="15" customHeight="1" spans="1:5">
       <c r="A18" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="32" t="s">
-        <v>21</v>
-      </c>
+      <c r="B18" s="32"/>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
       <c r="E18" s="49"/>
     </row>
     <row r="19" ht="15" customHeight="1" spans="1:5">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="34"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" ht="15" customHeight="1" spans="1:5">
+      <c r="A20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="50"/>
-    </row>
-    <row r="20" ht="15" customHeight="1" spans="1:5">
-      <c r="A20" s="25"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="1"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
     </row>
     <row r="21" ht="15" customHeight="1" spans="1:5">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
     </row>
     <row r="22" ht="15" customHeight="1" spans="1:5">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
     </row>
     <row r="23" ht="15" customHeight="1" spans="1:5">
       <c r="A23" s="17" t="s">
@@ -1968,28 +1890,26 @@
       <c r="A24" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+    </row>
+    <row r="25" ht="15" customHeight="1" spans="1:5">
+      <c r="A25" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-    </row>
-    <row r="25" ht="15" customHeight="1" spans="1:5">
-      <c r="A25" s="17" t="s">
+      <c r="B25" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
     </row>
     <row r="26" ht="15" customHeight="1" spans="1:5">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="40"/>
+      <c r="B26" s="38" t="s">
         <v>32</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>33</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -1998,7 +1918,7 @@
     <row r="27" ht="15" customHeight="1" spans="1:5">
       <c r="A27" s="40"/>
       <c r="B27" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>
@@ -2007,95 +1927,84 @@
     <row r="28" ht="15" customHeight="1" spans="1:5">
       <c r="A28" s="40"/>
       <c r="B28" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
     </row>
-    <row r="29" ht="15" customHeight="1" spans="1:5">
-      <c r="A29" s="40"/>
+    <row r="29" ht="14.25" customHeight="1" spans="1:5">
+      <c r="A29" s="40" t="s">
+        <v>35</v>
+      </c>
       <c r="B29" s="38" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="C29" s="38"/>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
     </row>
     <row r="30" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
     </row>
     <row r="31" ht="14.25" customHeight="1" spans="1:5">
       <c r="A31" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-    </row>
-    <row r="32" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A32" s="41" t="s">
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="21"/>
+    </row>
+    <row r="34" ht="17" spans="1:4">
+      <c r="A34" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B34" s="43"/>
+      <c r="C34" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="21"/>
-    </row>
-    <row r="35" ht="17" spans="1:4">
-      <c r="A35" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="45"/>
+      <c r="D34" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:E30"/>
     <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:E32"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B18:E19"/>
+    <mergeCell ref="B17:E18"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait"/>
   <headerFooter/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add confirm order api
</commit_message>
<xml_diff>
--- a/template/order_pi_template.xlsx
+++ b/template/order_pi_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26580" windowHeight="21760"/>
+    <workbookView windowWidth="23020" windowHeight="18760"/>
   </bookViews>
   <sheets>
     <sheet name="PI" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>NINGBO HARBOR IMPORT &amp; EXPORT CO.,LTD</t>
   </si>
@@ -94,27 +94,13 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">To:   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Real Flame Company Inc.</t>
+      <t>{{customer_name}}</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color indexed="56"/>
+        <color rgb="FF003366"/>
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
@@ -125,64 +111,25 @@
     <t>P/I NO.:</t>
   </si>
   <si>
-    <t>NBHB/RFC2331</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Add:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t>7800 Northwestern Avenue, Racine, WI 53406</t>
-    </r>
+    <t>{{pi_num}}</t>
+  </si>
+  <si>
+    <t>{{customer_address}}</t>
   </si>
   <si>
     <t>PO NO.:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Tel/Fax:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> 800 6541704</t>
-    </r>
+    <t>{{po_num}}</t>
+  </si>
+  <si>
+    <t>{{customer_tel_fax}}</t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
-    <t>2023.6.13</t>
+    <t>{{po_date}}</t>
   </si>
   <si>
     <t>Description</t>
@@ -212,7 +159,7 @@
     <t xml:space="preserve">1. TERMS OF PAYMENT:  </t>
   </si>
   <si>
-    <t>NO DEPOSIT. T/T WITHIN 21DAYS AFTER SHIPMENT</t>
+    <t>{{payment_method}}</t>
   </si>
   <si>
     <r>
@@ -234,7 +181,7 @@
     </r>
   </si>
   <si>
-    <t>AUG 18TH, 2023</t>
+    <t>{{delivery_date}}</t>
   </si>
   <si>
     <r>
@@ -256,7 +203,7 @@
     </r>
   </si>
   <si>
-    <t>NINGBO, CHINA</t>
+    <t>{{port_of_loading}}</t>
   </si>
   <si>
     <r>
@@ -289,7 +236,7 @@
     </r>
   </si>
   <si>
-    <t>MONTREAL, CANADA</t>
+    <t>{{port_of_destination}}</t>
   </si>
   <si>
     <t>5. BENEFICIARY’S BANK:</t>
@@ -603,7 +550,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color indexed="56"/>
+      <color rgb="FF003366"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -1651,8 +1598,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
@@ -1743,22 +1690,22 @@
       <c r="D9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="38">
-        <v>606234</v>
+      <c r="E9" s="38" t="s">
+        <v>10</v>
       </c>
       <c r="G9" s="46"/>
     </row>
     <row r="10" ht="15" customHeight="1" spans="1:7">
       <c r="A10" s="17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="12"/>
       <c r="D10" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G10" s="46"/>
     </row>
@@ -1784,19 +1731,19 @@
     </row>
     <row r="14" ht="15" customHeight="1" spans="1:7">
       <c r="A14" s="23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G14" s="46"/>
     </row>
@@ -1805,7 +1752,7 @@
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
       <c r="D15" s="24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" s="23"/>
       <c r="G15" s="46"/>
@@ -1819,7 +1766,7 @@
     </row>
     <row r="17" ht="15" customHeight="1" spans="1:5">
       <c r="A17" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="30"/>
@@ -1828,7 +1775,7 @@
     </row>
     <row r="18" ht="15" customHeight="1" spans="1:5">
       <c r="A18" s="31" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="32"/>
       <c r="C18" s="33"/>
@@ -1844,10 +1791,10 @@
     </row>
     <row r="20" ht="15" customHeight="1" spans="1:5">
       <c r="A20" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C20" s="36"/>
       <c r="D20" s="36"/>
@@ -1855,10 +1802,10 @@
     </row>
     <row r="21" ht="15" customHeight="1" spans="1:5">
       <c r="A21" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" s="37"/>
       <c r="D21" s="37"/>
@@ -1866,10 +1813,10 @@
     </row>
     <row r="22" ht="15" customHeight="1" spans="1:5">
       <c r="A22" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
@@ -1877,10 +1824,10 @@
     </row>
     <row r="23" ht="15" customHeight="1" spans="1:5">
       <c r="A23" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
@@ -1888,7 +1835,7 @@
     </row>
     <row r="24" ht="15" customHeight="1" spans="1:5">
       <c r="A24" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
@@ -1897,10 +1844,10 @@
     </row>
     <row r="25" ht="15" customHeight="1" spans="1:5">
       <c r="A25" s="38" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
@@ -1909,7 +1856,7 @@
     <row r="26" ht="15" customHeight="1" spans="1:5">
       <c r="A26" s="40"/>
       <c r="B26" s="38" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -1918,7 +1865,7 @@
     <row r="27" ht="15" customHeight="1" spans="1:5">
       <c r="A27" s="40"/>
       <c r="B27" s="38" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>
@@ -1927,7 +1874,7 @@
     <row r="28" ht="15" customHeight="1" spans="1:5">
       <c r="A28" s="40"/>
       <c r="B28" s="38" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
@@ -1935,7 +1882,7 @@
     </row>
     <row r="29" ht="14.25" customHeight="1" spans="1:5">
       <c r="A29" s="40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>0</v>
@@ -1946,10 +1893,10 @@
     </row>
     <row r="30" ht="14.25" customHeight="1" spans="1:5">
       <c r="A30" s="41" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" s="42"/>
       <c r="D30" s="42"/>
@@ -1957,10 +1904,10 @@
     </row>
     <row r="31" ht="14.25" customHeight="1" spans="1:5">
       <c r="A31" s="41" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C31" s="34"/>
       <c r="D31" s="34"/>
@@ -1971,11 +1918,11 @@
     </row>
     <row r="34" ht="17" spans="1:4">
       <c r="A34" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B34" s="43"/>
       <c r="C34" s="44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D34" s="45"/>
     </row>

</xml_diff>